<commit_message>
Add new event types
</commit_message>
<xml_diff>
--- a/RingetteSchedule/Master.xlsx
+++ b/RingetteSchedule/Master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5FD913-ED27-4A42-BCFE-5701E0DEC20F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA98A16F-A794-4D36-82C8-C7CC3B4EA61D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="163" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="163" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions" sheetId="7" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Season!$B:$B,Season!$3:$4</definedName>
-    <definedName name="Type">Season!$B$45:$B$49</definedName>
+    <definedName name="Type">Season!$B$45:$B$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="159">
   <si>
     <t>Sat</t>
   </si>
@@ -505,6 +505,12 @@
   <si>
     <t>Lasergirls (Alderwick)</t>
   </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T0.5</t>
+  </si>
 </sst>
 </file>
 
@@ -8593,12 +8599,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="94.109375" customWidth="1"/>
+    <col min="2" max="2" width="94.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>4</v>
       </c>
@@ -8606,7 +8612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -8614,29 +8620,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>56</v>
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H6" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="8"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
     </row>
   </sheetData>
@@ -8654,499 +8660,499 @@
   <dimension ref="A1:RM103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="DB59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="FD26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="DD74" sqref="DD74"/>
+      <selection pane="bottomRight" activeCell="FU38" sqref="FU38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="11" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="12" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="12" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="4.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="5.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="3.6640625" style="13" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" style="12" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" style="12" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="3.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5546875" style="4" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="4.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="18.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="4.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="16.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="4.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="16.5546875" style="4" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="3.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="16.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="3.6640625" style="13" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="18.88671875" style="12" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="4.5546875" style="4" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="17.109375" style="12" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="4.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="17.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="4.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="3.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="16.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="4.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="21.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="4.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="18.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="3.6640625" style="13" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="19.33203125" style="12" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="18.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="4.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="4.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="3.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="16.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="3.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" style="12" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="4.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="17.140625" style="12" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="4.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="17.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="4.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="3.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="16.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="4.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="21.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="4.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="18.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="3.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="19.28515625" style="12" hidden="1" customWidth="1"/>
     <col min="49" max="49" width="4" style="4" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="17.33203125" style="12" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="4.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="16.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="4.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="18.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="6.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="17.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" style="12" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="4.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="16.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="4.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="18.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="6.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="17.28515625" style="4" hidden="1" customWidth="1"/>
     <col min="57" max="57" width="5" style="1" hidden="1" customWidth="1"/>
     <col min="58" max="58" width="20" style="4" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="5.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="17.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="3.6640625" style="13" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="18.88671875" style="12" customWidth="1"/>
-    <col min="63" max="63" width="4.44140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="5.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="17.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="3.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="18.85546875" style="12" customWidth="1"/>
+    <col min="63" max="63" width="4.42578125" style="4" customWidth="1"/>
     <col min="64" max="64" width="18" style="12" customWidth="1"/>
-    <col min="65" max="65" width="4.109375" style="1" customWidth="1"/>
-    <col min="66" max="66" width="16.88671875" style="4" customWidth="1"/>
-    <col min="67" max="67" width="4.88671875" style="1" customWidth="1"/>
-    <col min="68" max="68" width="17.77734375" style="4" customWidth="1"/>
-    <col min="69" max="69" width="4.6640625" style="1" customWidth="1"/>
-    <col min="70" max="70" width="15.5546875" style="4" customWidth="1"/>
-    <col min="71" max="71" width="4.88671875" style="1" customWidth="1"/>
+    <col min="65" max="65" width="4.140625" style="1" customWidth="1"/>
+    <col min="66" max="66" width="16.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="4.85546875" style="1" customWidth="1"/>
+    <col min="68" max="68" width="17.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="4.7109375" style="1" customWidth="1"/>
+    <col min="70" max="70" width="15.5703125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="4.85546875" style="1" customWidth="1"/>
     <col min="72" max="72" width="21" style="4" customWidth="1"/>
-    <col min="73" max="73" width="4.44140625" style="1" customWidth="1"/>
-    <col min="74" max="74" width="15.6640625" style="4" customWidth="1"/>
-    <col min="75" max="75" width="6.44140625" style="13" customWidth="1"/>
-    <col min="76" max="76" width="18.5546875" style="12" customWidth="1"/>
-    <col min="77" max="77" width="4.44140625" style="4" customWidth="1"/>
+    <col min="73" max="73" width="4.42578125" style="1" customWidth="1"/>
+    <col min="74" max="74" width="15.7109375" style="4" customWidth="1"/>
+    <col min="75" max="75" width="6.42578125" style="13" customWidth="1"/>
+    <col min="76" max="76" width="18.5703125" style="12" customWidth="1"/>
+    <col min="77" max="77" width="4.42578125" style="4" customWidth="1"/>
     <col min="78" max="78" width="19" style="12" customWidth="1"/>
-    <col min="79" max="79" width="4.5546875" style="1" customWidth="1"/>
+    <col min="79" max="79" width="4.5703125" style="1" customWidth="1"/>
     <col min="80" max="80" width="17" style="4" customWidth="1"/>
     <col min="81" max="81" width="5" style="1" customWidth="1"/>
-    <col min="82" max="82" width="16.77734375" style="4" customWidth="1"/>
-    <col min="83" max="83" width="5.44140625" style="1" customWidth="1"/>
-    <col min="84" max="84" width="16.88671875" style="4" customWidth="1"/>
-    <col min="85" max="85" width="4.5546875" style="1" customWidth="1"/>
-    <col min="86" max="86" width="17.44140625" style="4" customWidth="1"/>
-    <col min="87" max="87" width="4.5546875" style="1" customWidth="1"/>
-    <col min="88" max="88" width="17.44140625" style="4" customWidth="1"/>
-    <col min="89" max="89" width="4.88671875" style="13" customWidth="1"/>
-    <col min="90" max="90" width="19.77734375" style="12" customWidth="1"/>
+    <col min="82" max="82" width="16.7109375" style="4" customWidth="1"/>
+    <col min="83" max="83" width="5.42578125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="16.85546875" style="4" customWidth="1"/>
+    <col min="85" max="85" width="4.5703125" style="1" customWidth="1"/>
+    <col min="86" max="86" width="17.42578125" style="4" customWidth="1"/>
+    <col min="87" max="87" width="4.5703125" style="1" customWidth="1"/>
+    <col min="88" max="88" width="17.42578125" style="4" customWidth="1"/>
+    <col min="89" max="89" width="4.85546875" style="13" customWidth="1"/>
+    <col min="90" max="90" width="19.7109375" style="12" customWidth="1"/>
     <col min="91" max="91" width="5" style="4" customWidth="1"/>
-    <col min="92" max="92" width="19.21875" style="12" customWidth="1"/>
-    <col min="93" max="93" width="5.88671875" style="1" customWidth="1"/>
-    <col min="94" max="94" width="18.44140625" style="4" customWidth="1"/>
-    <col min="95" max="95" width="4.5546875" style="1" customWidth="1"/>
-    <col min="96" max="96" width="17.109375" style="4" customWidth="1"/>
-    <col min="97" max="97" width="4.6640625" style="1" customWidth="1"/>
-    <col min="98" max="98" width="15.6640625" style="4" customWidth="1"/>
-    <col min="99" max="99" width="4.88671875" style="1" customWidth="1"/>
-    <col min="100" max="100" width="18.88671875" style="4" customWidth="1"/>
+    <col min="92" max="92" width="19.28515625" style="12" customWidth="1"/>
+    <col min="93" max="93" width="5.85546875" style="1" customWidth="1"/>
+    <col min="94" max="94" width="18.42578125" style="4" customWidth="1"/>
+    <col min="95" max="95" width="4.5703125" style="1" customWidth="1"/>
+    <col min="96" max="96" width="17.140625" style="4" customWidth="1"/>
+    <col min="97" max="97" width="4.7109375" style="1" customWidth="1"/>
+    <col min="98" max="98" width="15.7109375" style="4" customWidth="1"/>
+    <col min="99" max="99" width="4.85546875" style="1" customWidth="1"/>
+    <col min="100" max="100" width="18.85546875" style="4" customWidth="1"/>
     <col min="101" max="101" width="5" style="1" customWidth="1"/>
-    <col min="102" max="102" width="15.6640625" style="4" customWidth="1"/>
+    <col min="102" max="102" width="15.7109375" style="4" customWidth="1"/>
     <col min="103" max="103" width="7" style="13" customWidth="1"/>
-    <col min="104" max="104" width="18.44140625" style="12" customWidth="1"/>
+    <col min="104" max="104" width="18.42578125" style="12" customWidth="1"/>
     <col min="105" max="105" width="6" style="4" customWidth="1"/>
-    <col min="106" max="106" width="17.109375" style="12" customWidth="1"/>
-    <col min="107" max="107" width="4.88671875" style="1" customWidth="1"/>
-    <col min="108" max="108" width="15.6640625" style="4" customWidth="1"/>
-    <col min="109" max="109" width="5.21875" style="1" customWidth="1"/>
-    <col min="110" max="110" width="15.6640625" style="4" customWidth="1"/>
-    <col min="111" max="111" width="6.21875" style="1" customWidth="1"/>
-    <col min="112" max="112" width="15.6640625" style="4" customWidth="1"/>
-    <col min="113" max="113" width="5.109375" style="1" customWidth="1"/>
-    <col min="114" max="114" width="17.5546875" style="4" customWidth="1"/>
-    <col min="115" max="115" width="5.109375" style="1" customWidth="1"/>
-    <col min="116" max="116" width="15.6640625" style="4" customWidth="1"/>
-    <col min="117" max="117" width="5.21875" style="13" customWidth="1"/>
+    <col min="106" max="106" width="17.140625" style="12" customWidth="1"/>
+    <col min="107" max="107" width="4.85546875" style="1" customWidth="1"/>
+    <col min="108" max="108" width="15.7109375" style="4" customWidth="1"/>
+    <col min="109" max="109" width="5.28515625" style="1" customWidth="1"/>
+    <col min="110" max="110" width="15.7109375" style="4" customWidth="1"/>
+    <col min="111" max="111" width="6.28515625" style="1" customWidth="1"/>
+    <col min="112" max="112" width="15.7109375" style="4" customWidth="1"/>
+    <col min="113" max="113" width="5.140625" style="1" customWidth="1"/>
+    <col min="114" max="114" width="17.5703125" style="4" customWidth="1"/>
+    <col min="115" max="115" width="5.140625" style="1" customWidth="1"/>
+    <col min="116" max="116" width="15.7109375" style="4" customWidth="1"/>
+    <col min="117" max="117" width="5.28515625" style="13" customWidth="1"/>
     <col min="118" max="118" width="19" style="12" customWidth="1"/>
-    <col min="119" max="119" width="4.5546875" style="4" customWidth="1"/>
+    <col min="119" max="119" width="4.5703125" style="4" customWidth="1"/>
     <col min="120" max="120" width="24" style="12" customWidth="1"/>
-    <col min="121" max="121" width="4.44140625" style="1" customWidth="1"/>
-    <col min="122" max="122" width="19.21875" style="4" customWidth="1"/>
-    <col min="123" max="123" width="5.21875" style="1" customWidth="1"/>
-    <col min="124" max="124" width="15.6640625" style="4" customWidth="1"/>
-    <col min="125" max="125" width="5.6640625" style="1" customWidth="1"/>
-    <col min="126" max="126" width="15.6640625" style="4" customWidth="1"/>
+    <col min="121" max="121" width="4.42578125" style="1" customWidth="1"/>
+    <col min="122" max="122" width="19.28515625" style="4" customWidth="1"/>
+    <col min="123" max="123" width="5.28515625" style="1" customWidth="1"/>
+    <col min="124" max="124" width="15.7109375" style="4" customWidth="1"/>
+    <col min="125" max="125" width="5.7109375" style="1" customWidth="1"/>
+    <col min="126" max="126" width="15.7109375" style="4" customWidth="1"/>
     <col min="127" max="127" width="5" style="1" customWidth="1"/>
-    <col min="128" max="128" width="18.77734375" style="4" customWidth="1"/>
-    <col min="129" max="129" width="4.109375" style="1" customWidth="1"/>
-    <col min="130" max="130" width="15.6640625" style="4" customWidth="1"/>
-    <col min="131" max="131" width="5.109375" style="13" customWidth="1"/>
-    <col min="132" max="132" width="18.44140625" style="12" customWidth="1"/>
-    <col min="133" max="133" width="4.109375" style="4" customWidth="1"/>
-    <col min="134" max="134" width="23.33203125" style="12" customWidth="1"/>
-    <col min="135" max="135" width="4.44140625" style="1" customWidth="1"/>
-    <col min="136" max="136" width="15.6640625" style="4" customWidth="1"/>
-    <col min="137" max="137" width="4.88671875" style="1" customWidth="1"/>
-    <col min="138" max="138" width="15.6640625" style="4" customWidth="1"/>
-    <col min="139" max="139" width="3.6640625" style="1" customWidth="1"/>
-    <col min="140" max="140" width="15.6640625" style="4" customWidth="1"/>
-    <col min="141" max="141" width="4.5546875" style="1" customWidth="1"/>
-    <col min="142" max="142" width="17.44140625" style="4" customWidth="1"/>
-    <col min="143" max="143" width="4.33203125" style="1" customWidth="1"/>
-    <col min="144" max="144" width="15.6640625" style="4" customWidth="1"/>
-    <col min="145" max="145" width="3.6640625" style="13" customWidth="1"/>
-    <col min="146" max="146" width="19.33203125" style="12" customWidth="1"/>
-    <col min="147" max="147" width="4.109375" style="4" customWidth="1"/>
-    <col min="148" max="148" width="23.5546875" style="12" customWidth="1"/>
-    <col min="149" max="149" width="5.6640625" style="1" customWidth="1"/>
-    <col min="150" max="150" width="15.6640625" style="4" customWidth="1"/>
-    <col min="151" max="151" width="4.88671875" style="1" customWidth="1"/>
-    <col min="152" max="152" width="15.6640625" style="4" customWidth="1"/>
-    <col min="153" max="153" width="3.6640625" style="1" customWidth="1"/>
-    <col min="154" max="154" width="15.6640625" style="4" customWidth="1"/>
-    <col min="155" max="155" width="4.88671875" style="1" customWidth="1"/>
-    <col min="156" max="156" width="18.77734375" style="4" customWidth="1"/>
-    <col min="157" max="157" width="4.44140625" style="1" customWidth="1"/>
-    <col min="158" max="158" width="15.6640625" style="4" customWidth="1"/>
-    <col min="159" max="159" width="3.6640625" style="13" customWidth="1"/>
-    <col min="160" max="160" width="18.5546875" style="12" customWidth="1"/>
+    <col min="128" max="128" width="18.7109375" style="4" customWidth="1"/>
+    <col min="129" max="129" width="4.140625" style="1" customWidth="1"/>
+    <col min="130" max="130" width="15.7109375" style="4" customWidth="1"/>
+    <col min="131" max="131" width="5.140625" style="13" customWidth="1"/>
+    <col min="132" max="132" width="18.42578125" style="12" customWidth="1"/>
+    <col min="133" max="133" width="4.140625" style="4" customWidth="1"/>
+    <col min="134" max="134" width="23.28515625" style="12" customWidth="1"/>
+    <col min="135" max="135" width="4.42578125" style="1" customWidth="1"/>
+    <col min="136" max="136" width="15.7109375" style="4" customWidth="1"/>
+    <col min="137" max="137" width="4.85546875" style="1" customWidth="1"/>
+    <col min="138" max="138" width="15.7109375" style="4" customWidth="1"/>
+    <col min="139" max="139" width="3.7109375" style="1" customWidth="1"/>
+    <col min="140" max="140" width="15.7109375" style="4" customWidth="1"/>
+    <col min="141" max="141" width="4.5703125" style="1" customWidth="1"/>
+    <col min="142" max="142" width="17.42578125" style="4" customWidth="1"/>
+    <col min="143" max="143" width="4.28515625" style="1" customWidth="1"/>
+    <col min="144" max="144" width="15.7109375" style="4" customWidth="1"/>
+    <col min="145" max="145" width="3.7109375" style="13" customWidth="1"/>
+    <col min="146" max="146" width="19.28515625" style="12" customWidth="1"/>
+    <col min="147" max="147" width="4.140625" style="4" customWidth="1"/>
+    <col min="148" max="148" width="23.5703125" style="12" customWidth="1"/>
+    <col min="149" max="149" width="5.7109375" style="1" customWidth="1"/>
+    <col min="150" max="150" width="15.7109375" style="4" customWidth="1"/>
+    <col min="151" max="151" width="4.85546875" style="1" customWidth="1"/>
+    <col min="152" max="152" width="15.7109375" style="4" customWidth="1"/>
+    <col min="153" max="153" width="3.7109375" style="1" customWidth="1"/>
+    <col min="154" max="154" width="15.7109375" style="4" customWidth="1"/>
+    <col min="155" max="155" width="4.85546875" style="1" customWidth="1"/>
+    <col min="156" max="156" width="18.7109375" style="4" customWidth="1"/>
+    <col min="157" max="157" width="4.42578125" style="1" customWidth="1"/>
+    <col min="158" max="158" width="15.7109375" style="4" customWidth="1"/>
+    <col min="159" max="159" width="3.7109375" style="13" customWidth="1"/>
+    <col min="160" max="160" width="18.5703125" style="12" customWidth="1"/>
     <col min="161" max="161" width="5" style="4" customWidth="1"/>
-    <col min="162" max="162" width="23.88671875" style="12" customWidth="1"/>
-    <col min="163" max="163" width="5.33203125" style="1" customWidth="1"/>
-    <col min="164" max="164" width="15.6640625" style="4" customWidth="1"/>
-    <col min="165" max="165" width="5.21875" style="1" customWidth="1"/>
-    <col min="166" max="166" width="15.6640625" style="4" customWidth="1"/>
-    <col min="167" max="167" width="3.6640625" style="1" customWidth="1"/>
-    <col min="168" max="168" width="15.6640625" style="4" customWidth="1"/>
-    <col min="169" max="169" width="4.5546875" style="1" customWidth="1"/>
-    <col min="170" max="170" width="17.5546875" style="4" customWidth="1"/>
+    <col min="162" max="162" width="23.85546875" style="12" customWidth="1"/>
+    <col min="163" max="163" width="5.28515625" style="1" customWidth="1"/>
+    <col min="164" max="164" width="15.7109375" style="4" customWidth="1"/>
+    <col min="165" max="165" width="5.28515625" style="1" customWidth="1"/>
+    <col min="166" max="166" width="15.7109375" style="4" customWidth="1"/>
+    <col min="167" max="167" width="3.7109375" style="1" customWidth="1"/>
+    <col min="168" max="168" width="15.7109375" style="4" customWidth="1"/>
+    <col min="169" max="169" width="4.5703125" style="1" customWidth="1"/>
+    <col min="170" max="170" width="17.5703125" style="4" customWidth="1"/>
     <col min="171" max="171" width="5" style="1" customWidth="1"/>
-    <col min="172" max="172" width="15.6640625" style="4" customWidth="1"/>
-    <col min="173" max="173" width="3.6640625" style="13" customWidth="1"/>
-    <col min="174" max="174" width="18.44140625" style="12" customWidth="1"/>
-    <col min="175" max="175" width="5.109375" style="4" customWidth="1"/>
+    <col min="172" max="172" width="15.7109375" style="4" customWidth="1"/>
+    <col min="173" max="173" width="3.7109375" style="13" customWidth="1"/>
+    <col min="174" max="174" width="18.42578125" style="12" customWidth="1"/>
+    <col min="175" max="175" width="5.140625" style="4" customWidth="1"/>
     <col min="176" max="176" width="23" style="12" customWidth="1"/>
-    <col min="177" max="177" width="4.5546875" style="1" customWidth="1"/>
-    <col min="178" max="178" width="15.6640625" style="4" customWidth="1"/>
-    <col min="179" max="179" width="3.6640625" style="1" customWidth="1"/>
-    <col min="180" max="180" width="15.6640625" style="4" customWidth="1"/>
-    <col min="181" max="181" width="3.6640625" style="1" customWidth="1"/>
-    <col min="182" max="182" width="15.6640625" style="4" customWidth="1"/>
-    <col min="183" max="183" width="4.44140625" style="1" customWidth="1"/>
-    <col min="184" max="184" width="17.109375" style="4" customWidth="1"/>
-    <col min="185" max="185" width="4.6640625" style="1" customWidth="1"/>
-    <col min="186" max="186" width="17.33203125" style="4" customWidth="1"/>
-    <col min="187" max="187" width="3.6640625" style="13" customWidth="1"/>
-    <col min="188" max="188" width="19.109375" style="12" customWidth="1"/>
-    <col min="189" max="189" width="4.88671875" style="4" customWidth="1"/>
-    <col min="190" max="190" width="23.6640625" style="12" customWidth="1"/>
-    <col min="191" max="191" width="4.44140625" style="1" customWidth="1"/>
-    <col min="192" max="192" width="15.6640625" style="4" customWidth="1"/>
-    <col min="193" max="193" width="3.6640625" style="1" customWidth="1"/>
-    <col min="194" max="194" width="15.6640625" style="4" customWidth="1"/>
-    <col min="195" max="195" width="3.6640625" style="1" customWidth="1"/>
-    <col min="196" max="196" width="15.6640625" style="4" customWidth="1"/>
+    <col min="177" max="177" width="4.5703125" style="1" customWidth="1"/>
+    <col min="178" max="178" width="15.7109375" style="4" customWidth="1"/>
+    <col min="179" max="179" width="3.7109375" style="1" customWidth="1"/>
+    <col min="180" max="180" width="15.7109375" style="4" customWidth="1"/>
+    <col min="181" max="181" width="3.7109375" style="1" customWidth="1"/>
+    <col min="182" max="182" width="15.7109375" style="4" customWidth="1"/>
+    <col min="183" max="183" width="4.42578125" style="1" customWidth="1"/>
+    <col min="184" max="184" width="17.140625" style="4" customWidth="1"/>
+    <col min="185" max="185" width="4.7109375" style="1" customWidth="1"/>
+    <col min="186" max="186" width="17.28515625" style="4" customWidth="1"/>
+    <col min="187" max="187" width="3.7109375" style="13" customWidth="1"/>
+    <col min="188" max="188" width="19.140625" style="12" customWidth="1"/>
+    <col min="189" max="189" width="4.85546875" style="4" customWidth="1"/>
+    <col min="190" max="190" width="23.7109375" style="12" customWidth="1"/>
+    <col min="191" max="191" width="4.42578125" style="1" customWidth="1"/>
+    <col min="192" max="192" width="15.7109375" style="4" customWidth="1"/>
+    <col min="193" max="193" width="3.7109375" style="1" customWidth="1"/>
+    <col min="194" max="194" width="15.7109375" style="4" customWidth="1"/>
+    <col min="195" max="195" width="3.7109375" style="1" customWidth="1"/>
+    <col min="196" max="196" width="15.7109375" style="4" customWidth="1"/>
     <col min="197" max="197" width="5" style="1" customWidth="1"/>
-    <col min="198" max="198" width="19.33203125" style="4" customWidth="1"/>
-    <col min="199" max="199" width="5.33203125" style="1" customWidth="1"/>
-    <col min="200" max="200" width="15.6640625" style="4" customWidth="1"/>
-    <col min="201" max="201" width="3.6640625" style="13" customWidth="1"/>
-    <col min="202" max="202" width="19.6640625" style="12" customWidth="1"/>
-    <col min="203" max="203" width="5.21875" style="4" customWidth="1"/>
-    <col min="204" max="204" width="23.5546875" style="12" customWidth="1"/>
-    <col min="205" max="205" width="5.44140625" style="1" customWidth="1"/>
-    <col min="206" max="206" width="15.6640625" style="4" customWidth="1"/>
-    <col min="207" max="207" width="3.6640625" style="1" customWidth="1"/>
-    <col min="208" max="208" width="15.6640625" style="4" customWidth="1"/>
-    <col min="209" max="209" width="3.6640625" style="1" customWidth="1"/>
-    <col min="210" max="210" width="15.6640625" style="4" customWidth="1"/>
-    <col min="211" max="211" width="4.44140625" style="1" customWidth="1"/>
-    <col min="212" max="212" width="16.33203125" style="4" customWidth="1"/>
+    <col min="198" max="198" width="19.28515625" style="4" customWidth="1"/>
+    <col min="199" max="199" width="5.28515625" style="1" customWidth="1"/>
+    <col min="200" max="200" width="15.7109375" style="4" customWidth="1"/>
+    <col min="201" max="201" width="3.7109375" style="13" customWidth="1"/>
+    <col min="202" max="202" width="19.7109375" style="12" customWidth="1"/>
+    <col min="203" max="203" width="5.28515625" style="4" customWidth="1"/>
+    <col min="204" max="204" width="23.5703125" style="12" customWidth="1"/>
+    <col min="205" max="205" width="5.42578125" style="1" customWidth="1"/>
+    <col min="206" max="206" width="15.7109375" style="4" customWidth="1"/>
+    <col min="207" max="207" width="3.7109375" style="1" customWidth="1"/>
+    <col min="208" max="208" width="15.7109375" style="4" customWidth="1"/>
+    <col min="209" max="209" width="3.7109375" style="1" customWidth="1"/>
+    <col min="210" max="210" width="15.7109375" style="4" customWidth="1"/>
+    <col min="211" max="211" width="4.42578125" style="1" customWidth="1"/>
+    <col min="212" max="212" width="16.28515625" style="4" customWidth="1"/>
     <col min="213" max="213" width="5" style="1" customWidth="1"/>
-    <col min="214" max="214" width="15.6640625" style="4" customWidth="1"/>
-    <col min="215" max="215" width="3.6640625" style="13" customWidth="1"/>
+    <col min="214" max="214" width="15.7109375" style="4" customWidth="1"/>
+    <col min="215" max="215" width="3.7109375" style="13" customWidth="1"/>
     <col min="216" max="216" width="19" style="12" customWidth="1"/>
-    <col min="217" max="217" width="5.88671875" style="4" customWidth="1"/>
-    <col min="218" max="218" width="23.6640625" style="12" customWidth="1"/>
-    <col min="219" max="219" width="4.5546875" style="1" customWidth="1"/>
-    <col min="220" max="220" width="15.6640625" style="4" customWidth="1"/>
-    <col min="221" max="221" width="3.6640625" style="1" customWidth="1"/>
-    <col min="222" max="222" width="15.6640625" style="4" customWidth="1"/>
-    <col min="223" max="223" width="3.6640625" style="1" customWidth="1"/>
-    <col min="224" max="224" width="15.6640625" style="4" customWidth="1"/>
-    <col min="225" max="225" width="4.44140625" style="1" customWidth="1"/>
-    <col min="226" max="226" width="17.109375" style="4" customWidth="1"/>
-    <col min="227" max="227" width="5.5546875" style="1" customWidth="1"/>
-    <col min="228" max="228" width="15.6640625" style="4" customWidth="1"/>
-    <col min="229" max="229" width="3.6640625" style="13" customWidth="1"/>
-    <col min="230" max="230" width="18.33203125" style="12" customWidth="1"/>
-    <col min="231" max="231" width="5.109375" style="4" customWidth="1"/>
-    <col min="232" max="232" width="23.44140625" style="12" customWidth="1"/>
-    <col min="233" max="233" width="4.44140625" style="1" customWidth="1"/>
-    <col min="234" max="234" width="15.6640625" style="4" customWidth="1"/>
-    <col min="235" max="235" width="5.21875" style="1" customWidth="1"/>
-    <col min="236" max="236" width="15.6640625" style="4" customWidth="1"/>
-    <col min="237" max="237" width="3.6640625" style="1" customWidth="1"/>
-    <col min="238" max="238" width="15.6640625" style="4" customWidth="1"/>
+    <col min="217" max="217" width="5.85546875" style="4" customWidth="1"/>
+    <col min="218" max="218" width="23.7109375" style="12" customWidth="1"/>
+    <col min="219" max="219" width="4.5703125" style="1" customWidth="1"/>
+    <col min="220" max="220" width="15.7109375" style="4" customWidth="1"/>
+    <col min="221" max="221" width="3.7109375" style="1" customWidth="1"/>
+    <col min="222" max="222" width="15.7109375" style="4" customWidth="1"/>
+    <col min="223" max="223" width="3.7109375" style="1" customWidth="1"/>
+    <col min="224" max="224" width="15.7109375" style="4" customWidth="1"/>
+    <col min="225" max="225" width="4.42578125" style="1" customWidth="1"/>
+    <col min="226" max="226" width="17.140625" style="4" customWidth="1"/>
+    <col min="227" max="227" width="5.5703125" style="1" customWidth="1"/>
+    <col min="228" max="228" width="15.7109375" style="4" customWidth="1"/>
+    <col min="229" max="229" width="3.7109375" style="13" customWidth="1"/>
+    <col min="230" max="230" width="18.28515625" style="12" customWidth="1"/>
+    <col min="231" max="231" width="5.140625" style="4" customWidth="1"/>
+    <col min="232" max="232" width="23.42578125" style="12" customWidth="1"/>
+    <col min="233" max="233" width="4.42578125" style="1" customWidth="1"/>
+    <col min="234" max="234" width="15.7109375" style="4" customWidth="1"/>
+    <col min="235" max="235" width="5.28515625" style="1" customWidth="1"/>
+    <col min="236" max="236" width="15.7109375" style="4" customWidth="1"/>
+    <col min="237" max="237" width="3.7109375" style="1" customWidth="1"/>
+    <col min="238" max="238" width="15.7109375" style="4" customWidth="1"/>
     <col min="239" max="239" width="5" style="1" customWidth="1"/>
     <col min="240" max="240" width="20" style="4" customWidth="1"/>
-    <col min="241" max="241" width="5.21875" style="1" customWidth="1"/>
-    <col min="242" max="242" width="15.6640625" style="4" customWidth="1"/>
-    <col min="243" max="243" width="3.6640625" style="13" customWidth="1"/>
+    <col min="241" max="241" width="5.28515625" style="1" customWidth="1"/>
+    <col min="242" max="242" width="15.7109375" style="4" customWidth="1"/>
+    <col min="243" max="243" width="3.7109375" style="13" customWidth="1"/>
     <col min="244" max="244" width="19" style="12" customWidth="1"/>
-    <col min="245" max="245" width="5.77734375" style="4" customWidth="1"/>
-    <col min="246" max="246" width="23.33203125" style="12" customWidth="1"/>
-    <col min="247" max="247" width="6.33203125" style="1" customWidth="1"/>
-    <col min="248" max="248" width="19.44140625" style="4" customWidth="1"/>
+    <col min="245" max="245" width="5.7109375" style="4" customWidth="1"/>
+    <col min="246" max="246" width="23.28515625" style="12" customWidth="1"/>
+    <col min="247" max="247" width="6.28515625" style="1" customWidth="1"/>
+    <col min="248" max="248" width="19.42578125" style="4" customWidth="1"/>
     <col min="249" max="249" width="5" style="1" customWidth="1"/>
-    <col min="250" max="250" width="15.6640625" style="4" customWidth="1"/>
-    <col min="251" max="251" width="3.6640625" style="1" customWidth="1"/>
-    <col min="252" max="252" width="17.6640625" style="4" customWidth="1"/>
-    <col min="253" max="253" width="4.44140625" style="1" customWidth="1"/>
-    <col min="254" max="254" width="18.44140625" style="4" customWidth="1"/>
-    <col min="255" max="255" width="3.6640625" style="1" customWidth="1"/>
-    <col min="256" max="256" width="15.6640625" style="4" customWidth="1"/>
-    <col min="257" max="257" width="3.6640625" style="13"/>
-    <col min="258" max="258" width="18.44140625" style="12" customWidth="1"/>
-    <col min="259" max="259" width="4.44140625" style="4" customWidth="1"/>
+    <col min="250" max="250" width="15.7109375" style="4" customWidth="1"/>
+    <col min="251" max="251" width="3.7109375" style="1" customWidth="1"/>
+    <col min="252" max="252" width="17.7109375" style="4" customWidth="1"/>
+    <col min="253" max="253" width="4.42578125" style="1" customWidth="1"/>
+    <col min="254" max="254" width="18.42578125" style="4" customWidth="1"/>
+    <col min="255" max="255" width="3.7109375" style="1" customWidth="1"/>
+    <col min="256" max="256" width="15.7109375" style="4" customWidth="1"/>
+    <col min="257" max="257" width="3.7109375" style="13"/>
+    <col min="258" max="258" width="18.42578125" style="12" customWidth="1"/>
+    <col min="259" max="259" width="4.42578125" style="4" customWidth="1"/>
     <col min="260" max="260" width="20" style="12" customWidth="1"/>
-    <col min="261" max="261" width="5.33203125" style="1" customWidth="1"/>
-    <col min="262" max="262" width="15.6640625" style="4" customWidth="1"/>
-    <col min="263" max="263" width="3.6640625" style="1" customWidth="1"/>
-    <col min="264" max="264" width="15.6640625" style="4" customWidth="1"/>
-    <col min="265" max="265" width="3.6640625" style="1" customWidth="1"/>
-    <col min="266" max="266" width="15.6640625" style="4" customWidth="1"/>
-    <col min="267" max="267" width="4.88671875" style="1" customWidth="1"/>
-    <col min="268" max="268" width="16.6640625" style="4" customWidth="1"/>
-    <col min="269" max="269" width="3.88671875" style="1" customWidth="1"/>
-    <col min="270" max="270" width="15.6640625" style="4" customWidth="1"/>
-    <col min="271" max="271" width="3.6640625" style="13" customWidth="1"/>
-    <col min="272" max="272" width="19.6640625" style="12" customWidth="1"/>
-    <col min="273" max="273" width="4.6640625" style="4" customWidth="1"/>
+    <col min="261" max="261" width="5.28515625" style="1" customWidth="1"/>
+    <col min="262" max="262" width="15.7109375" style="4" customWidth="1"/>
+    <col min="263" max="263" width="3.7109375" style="1" customWidth="1"/>
+    <col min="264" max="264" width="15.7109375" style="4" customWidth="1"/>
+    <col min="265" max="265" width="3.7109375" style="1" customWidth="1"/>
+    <col min="266" max="266" width="15.7109375" style="4" customWidth="1"/>
+    <col min="267" max="267" width="4.85546875" style="1" customWidth="1"/>
+    <col min="268" max="268" width="16.7109375" style="4" customWidth="1"/>
+    <col min="269" max="269" width="3.85546875" style="1" customWidth="1"/>
+    <col min="270" max="270" width="15.7109375" style="4" customWidth="1"/>
+    <col min="271" max="271" width="3.7109375" style="13" customWidth="1"/>
+    <col min="272" max="272" width="19.7109375" style="12" customWidth="1"/>
+    <col min="273" max="273" width="4.7109375" style="4" customWidth="1"/>
     <col min="274" max="274" width="24" style="12" customWidth="1"/>
-    <col min="275" max="275" width="4.88671875" style="1" customWidth="1"/>
-    <col min="276" max="276" width="15.6640625" style="4" customWidth="1"/>
-    <col min="277" max="277" width="3.6640625" style="1" customWidth="1"/>
-    <col min="278" max="278" width="15.6640625" style="4" customWidth="1"/>
-    <col min="279" max="279" width="3.6640625" style="1" customWidth="1"/>
-    <col min="280" max="280" width="15.6640625" style="4" customWidth="1"/>
+    <col min="275" max="275" width="4.85546875" style="1" customWidth="1"/>
+    <col min="276" max="276" width="15.7109375" style="4" customWidth="1"/>
+    <col min="277" max="277" width="3.7109375" style="1" customWidth="1"/>
+    <col min="278" max="278" width="15.7109375" style="4" customWidth="1"/>
+    <col min="279" max="279" width="3.7109375" style="1" customWidth="1"/>
+    <col min="280" max="280" width="15.7109375" style="4" customWidth="1"/>
     <col min="281" max="281" width="5" style="1" customWidth="1"/>
     <col min="282" max="282" width="17" style="4" customWidth="1"/>
-    <col min="283" max="283" width="4.6640625" style="1" customWidth="1"/>
-    <col min="284" max="284" width="15.6640625" style="4" customWidth="1"/>
-    <col min="285" max="285" width="3.6640625" style="13" customWidth="1"/>
-    <col min="286" max="286" width="18.44140625" style="12" customWidth="1"/>
-    <col min="287" max="287" width="4.44140625" style="4" customWidth="1"/>
-    <col min="288" max="288" width="23.6640625" style="12" customWidth="1"/>
-    <col min="289" max="289" width="4.44140625" style="1" customWidth="1"/>
-    <col min="290" max="290" width="15.6640625" style="4" customWidth="1"/>
-    <col min="291" max="291" width="3.6640625" style="1" customWidth="1"/>
-    <col min="292" max="292" width="15.6640625" style="4" customWidth="1"/>
-    <col min="293" max="293" width="3.6640625" style="1" customWidth="1"/>
-    <col min="294" max="294" width="15.6640625" style="4" customWidth="1"/>
-    <col min="295" max="295" width="4.6640625" style="1" customWidth="1"/>
-    <col min="296" max="296" width="16.6640625" style="4" customWidth="1"/>
-    <col min="297" max="297" width="4.6640625" style="1" customWidth="1"/>
-    <col min="298" max="298" width="15.6640625" style="4" customWidth="1"/>
-    <col min="299" max="299" width="3.6640625" style="13" customWidth="1"/>
-    <col min="300" max="300" width="18.44140625" style="12" customWidth="1"/>
+    <col min="283" max="283" width="4.7109375" style="1" customWidth="1"/>
+    <col min="284" max="284" width="15.7109375" style="4" customWidth="1"/>
+    <col min="285" max="285" width="3.7109375" style="13" customWidth="1"/>
+    <col min="286" max="286" width="18.42578125" style="12" customWidth="1"/>
+    <col min="287" max="287" width="4.42578125" style="4" customWidth="1"/>
+    <col min="288" max="288" width="23.7109375" style="12" customWidth="1"/>
+    <col min="289" max="289" width="4.42578125" style="1" customWidth="1"/>
+    <col min="290" max="290" width="15.7109375" style="4" customWidth="1"/>
+    <col min="291" max="291" width="3.7109375" style="1" customWidth="1"/>
+    <col min="292" max="292" width="15.7109375" style="4" customWidth="1"/>
+    <col min="293" max="293" width="3.7109375" style="1" customWidth="1"/>
+    <col min="294" max="294" width="15.7109375" style="4" customWidth="1"/>
+    <col min="295" max="295" width="4.7109375" style="1" customWidth="1"/>
+    <col min="296" max="296" width="16.7109375" style="4" customWidth="1"/>
+    <col min="297" max="297" width="4.7109375" style="1" customWidth="1"/>
+    <col min="298" max="298" width="15.7109375" style="4" customWidth="1"/>
+    <col min="299" max="299" width="3.7109375" style="13" customWidth="1"/>
+    <col min="300" max="300" width="18.42578125" style="12" customWidth="1"/>
     <col min="301" max="301" width="5" style="4" customWidth="1"/>
-    <col min="302" max="302" width="23.33203125" style="12" customWidth="1"/>
-    <col min="303" max="303" width="4.6640625" style="1" customWidth="1"/>
-    <col min="304" max="304" width="15.6640625" style="4" customWidth="1"/>
-    <col min="305" max="305" width="3.6640625" style="1" customWidth="1"/>
-    <col min="306" max="306" width="15.6640625" style="4" customWidth="1"/>
-    <col min="307" max="307" width="3.6640625" style="1" customWidth="1"/>
-    <col min="308" max="308" width="15.6640625" style="4" customWidth="1"/>
-    <col min="309" max="309" width="4.6640625" style="1" customWidth="1"/>
-    <col min="310" max="310" width="16.88671875" style="4" customWidth="1"/>
-    <col min="311" max="311" width="4.88671875" style="1" customWidth="1"/>
-    <col min="312" max="312" width="15.6640625" style="4" customWidth="1"/>
-    <col min="313" max="313" width="3.6640625" style="13" customWidth="1"/>
-    <col min="314" max="314" width="18.44140625" style="12" customWidth="1"/>
-    <col min="315" max="315" width="4.6640625" style="4" customWidth="1"/>
-    <col min="316" max="316" width="24.109375" style="12" customWidth="1"/>
-    <col min="317" max="317" width="4.44140625" style="1" customWidth="1"/>
-    <col min="318" max="318" width="15.6640625" style="4" customWidth="1"/>
-    <col min="319" max="319" width="3.6640625" style="1" customWidth="1"/>
-    <col min="320" max="320" width="15.6640625" style="4" customWidth="1"/>
-    <col min="321" max="321" width="3.6640625" style="1" customWidth="1"/>
-    <col min="322" max="322" width="15.6640625" style="4" customWidth="1"/>
-    <col min="323" max="323" width="4.33203125" style="1" customWidth="1"/>
-    <col min="324" max="324" width="16.6640625" style="4" customWidth="1"/>
-    <col min="325" max="325" width="4.44140625" style="1" customWidth="1"/>
-    <col min="326" max="326" width="15.6640625" style="4" customWidth="1"/>
-    <col min="327" max="327" width="3.6640625" style="13" customWidth="1"/>
-    <col min="328" max="328" width="18.44140625" style="12" customWidth="1"/>
-    <col min="329" max="329" width="4.6640625" style="4" customWidth="1"/>
-    <col min="330" max="330" width="24.6640625" style="12" customWidth="1"/>
-    <col min="331" max="331" width="4.6640625" style="1" customWidth="1"/>
-    <col min="332" max="332" width="15.6640625" style="4" customWidth="1"/>
+    <col min="302" max="302" width="23.28515625" style="12" customWidth="1"/>
+    <col min="303" max="303" width="4.7109375" style="1" customWidth="1"/>
+    <col min="304" max="304" width="15.7109375" style="4" customWidth="1"/>
+    <col min="305" max="305" width="3.7109375" style="1" customWidth="1"/>
+    <col min="306" max="306" width="15.7109375" style="4" customWidth="1"/>
+    <col min="307" max="307" width="3.7109375" style="1" customWidth="1"/>
+    <col min="308" max="308" width="15.7109375" style="4" customWidth="1"/>
+    <col min="309" max="309" width="4.7109375" style="1" customWidth="1"/>
+    <col min="310" max="310" width="16.85546875" style="4" customWidth="1"/>
+    <col min="311" max="311" width="4.85546875" style="1" customWidth="1"/>
+    <col min="312" max="312" width="15.7109375" style="4" customWidth="1"/>
+    <col min="313" max="313" width="3.7109375" style="13" customWidth="1"/>
+    <col min="314" max="314" width="18.42578125" style="12" customWidth="1"/>
+    <col min="315" max="315" width="4.7109375" style="4" customWidth="1"/>
+    <col min="316" max="316" width="24.140625" style="12" customWidth="1"/>
+    <col min="317" max="317" width="4.42578125" style="1" customWidth="1"/>
+    <col min="318" max="318" width="15.7109375" style="4" customWidth="1"/>
+    <col min="319" max="319" width="3.7109375" style="1" customWidth="1"/>
+    <col min="320" max="320" width="15.7109375" style="4" customWidth="1"/>
+    <col min="321" max="321" width="3.7109375" style="1" customWidth="1"/>
+    <col min="322" max="322" width="15.7109375" style="4" customWidth="1"/>
+    <col min="323" max="323" width="4.28515625" style="1" customWidth="1"/>
+    <col min="324" max="324" width="16.7109375" style="4" customWidth="1"/>
+    <col min="325" max="325" width="4.42578125" style="1" customWidth="1"/>
+    <col min="326" max="326" width="15.7109375" style="4" customWidth="1"/>
+    <col min="327" max="327" width="3.7109375" style="13" customWidth="1"/>
+    <col min="328" max="328" width="18.42578125" style="12" customWidth="1"/>
+    <col min="329" max="329" width="4.7109375" style="4" customWidth="1"/>
+    <col min="330" max="330" width="24.7109375" style="12" customWidth="1"/>
+    <col min="331" max="331" width="4.7109375" style="1" customWidth="1"/>
+    <col min="332" max="332" width="15.7109375" style="4" customWidth="1"/>
     <col min="333" max="333" width="5" style="1" customWidth="1"/>
-    <col min="334" max="334" width="15.6640625" style="4" customWidth="1"/>
+    <col min="334" max="334" width="15.7109375" style="4" customWidth="1"/>
     <col min="335" max="335" width="4" style="1" customWidth="1"/>
-    <col min="336" max="336" width="15.6640625" style="4" customWidth="1"/>
-    <col min="337" max="337" width="4.88671875" style="1" customWidth="1"/>
-    <col min="338" max="338" width="16.6640625" style="4" customWidth="1"/>
-    <col min="339" max="339" width="5.33203125" style="1" customWidth="1"/>
-    <col min="340" max="340" width="15.6640625" style="4" customWidth="1"/>
-    <col min="341" max="341" width="4.44140625" style="13" customWidth="1"/>
+    <col min="336" max="336" width="15.7109375" style="4" customWidth="1"/>
+    <col min="337" max="337" width="4.85546875" style="1" customWidth="1"/>
+    <col min="338" max="338" width="16.7109375" style="4" customWidth="1"/>
+    <col min="339" max="339" width="5.28515625" style="1" customWidth="1"/>
+    <col min="340" max="340" width="15.7109375" style="4" customWidth="1"/>
+    <col min="341" max="341" width="4.42578125" style="13" customWidth="1"/>
     <col min="342" max="342" width="19" style="12" customWidth="1"/>
-    <col min="343" max="343" width="5.33203125" style="4" customWidth="1"/>
+    <col min="343" max="343" width="5.28515625" style="4" customWidth="1"/>
     <col min="344" max="344" width="25" style="12" customWidth="1"/>
     <col min="345" max="345" width="5" style="1" customWidth="1"/>
-    <col min="346" max="346" width="15.6640625" style="4" customWidth="1"/>
-    <col min="347" max="347" width="4.88671875" style="1" customWidth="1"/>
-    <col min="348" max="348" width="15.6640625" style="4" customWidth="1"/>
-    <col min="349" max="349" width="3.6640625" style="1" customWidth="1"/>
-    <col min="350" max="350" width="15.6640625" style="4" customWidth="1"/>
-    <col min="351" max="351" width="4.44140625" style="1" customWidth="1"/>
-    <col min="352" max="352" width="15.6640625" style="4" customWidth="1"/>
-    <col min="353" max="353" width="4.6640625" style="1" customWidth="1"/>
-    <col min="354" max="354" width="15.6640625" style="4" customWidth="1"/>
-    <col min="355" max="355" width="3.6640625" style="13" customWidth="1"/>
-    <col min="356" max="356" width="18.44140625" style="12" customWidth="1"/>
+    <col min="346" max="346" width="15.7109375" style="4" customWidth="1"/>
+    <col min="347" max="347" width="4.85546875" style="1" customWidth="1"/>
+    <col min="348" max="348" width="15.7109375" style="4" customWidth="1"/>
+    <col min="349" max="349" width="3.7109375" style="1" customWidth="1"/>
+    <col min="350" max="350" width="15.7109375" style="4" customWidth="1"/>
+    <col min="351" max="351" width="4.42578125" style="1" customWidth="1"/>
+    <col min="352" max="352" width="15.7109375" style="4" customWidth="1"/>
+    <col min="353" max="353" width="4.7109375" style="1" customWidth="1"/>
+    <col min="354" max="354" width="15.7109375" style="4" customWidth="1"/>
+    <col min="355" max="355" width="3.7109375" style="13" customWidth="1"/>
+    <col min="356" max="356" width="18.42578125" style="12" customWidth="1"/>
     <col min="357" max="357" width="5" style="4" customWidth="1"/>
-    <col min="358" max="358" width="23.109375" style="12" customWidth="1"/>
-    <col min="359" max="359" width="4.6640625" style="1" customWidth="1"/>
-    <col min="360" max="360" width="15.6640625" style="4" customWidth="1"/>
-    <col min="361" max="361" width="4.33203125" style="1" customWidth="1"/>
-    <col min="362" max="362" width="15.6640625" style="4" customWidth="1"/>
-    <col min="363" max="363" width="3.6640625" style="1" customWidth="1"/>
-    <col min="364" max="364" width="16.33203125" style="4" customWidth="1"/>
-    <col min="365" max="365" width="4.44140625" style="1" customWidth="1"/>
-    <col min="366" max="366" width="16.5546875" style="4" customWidth="1"/>
-    <col min="367" max="367" width="4.6640625" style="1" customWidth="1"/>
-    <col min="368" max="368" width="15.6640625" style="4" customWidth="1"/>
-    <col min="369" max="369" width="3.6640625" style="13" customWidth="1"/>
-    <col min="370" max="370" width="19.33203125" style="12" customWidth="1"/>
-    <col min="371" max="371" width="4.88671875" style="4" customWidth="1"/>
-    <col min="372" max="372" width="23.44140625" style="12" customWidth="1"/>
-    <col min="373" max="373" width="4.88671875" style="1" customWidth="1"/>
-    <col min="374" max="374" width="15.6640625" style="4" customWidth="1"/>
+    <col min="358" max="358" width="23.140625" style="12" customWidth="1"/>
+    <col min="359" max="359" width="4.7109375" style="1" customWidth="1"/>
+    <col min="360" max="360" width="15.7109375" style="4" customWidth="1"/>
+    <col min="361" max="361" width="4.28515625" style="1" customWidth="1"/>
+    <col min="362" max="362" width="15.7109375" style="4" customWidth="1"/>
+    <col min="363" max="363" width="3.7109375" style="1" customWidth="1"/>
+    <col min="364" max="364" width="16.28515625" style="4" customWidth="1"/>
+    <col min="365" max="365" width="4.42578125" style="1" customWidth="1"/>
+    <col min="366" max="366" width="16.5703125" style="4" customWidth="1"/>
+    <col min="367" max="367" width="4.7109375" style="1" customWidth="1"/>
+    <col min="368" max="368" width="15.7109375" style="4" customWidth="1"/>
+    <col min="369" max="369" width="3.7109375" style="13" customWidth="1"/>
+    <col min="370" max="370" width="19.28515625" style="12" customWidth="1"/>
+    <col min="371" max="371" width="4.85546875" style="4" customWidth="1"/>
+    <col min="372" max="372" width="23.42578125" style="12" customWidth="1"/>
+    <col min="373" max="373" width="4.85546875" style="1" customWidth="1"/>
+    <col min="374" max="374" width="15.7109375" style="4" customWidth="1"/>
     <col min="375" max="375" width="5" style="1" customWidth="1"/>
-    <col min="376" max="376" width="15.6640625" style="4" customWidth="1"/>
-    <col min="377" max="377" width="3.6640625" style="1" customWidth="1"/>
-    <col min="378" max="378" width="15.6640625" style="4" customWidth="1"/>
+    <col min="376" max="376" width="15.7109375" style="4" customWidth="1"/>
+    <col min="377" max="377" width="3.7109375" style="1" customWidth="1"/>
+    <col min="378" max="378" width="15.7109375" style="4" customWidth="1"/>
     <col min="379" max="379" width="5" style="1" customWidth="1"/>
-    <col min="380" max="380" width="17.33203125" style="4" customWidth="1"/>
-    <col min="381" max="381" width="4.88671875" style="1" customWidth="1"/>
-    <col min="382" max="382" width="15.6640625" style="4" customWidth="1"/>
-    <col min="383" max="383" width="3.6640625" style="13" customWidth="1"/>
-    <col min="384" max="384" width="18.5546875" style="12" customWidth="1"/>
-    <col min="385" max="385" width="4.88671875" style="4" customWidth="1"/>
-    <col min="386" max="386" width="15.6640625" style="12" customWidth="1"/>
-    <col min="387" max="387" width="3.6640625" style="1" customWidth="1"/>
-    <col min="388" max="388" width="15.6640625" style="4" customWidth="1"/>
-    <col min="389" max="389" width="5.44140625" style="1" customWidth="1"/>
-    <col min="390" max="390" width="15.6640625" style="4" customWidth="1"/>
-    <col min="391" max="391" width="3.6640625" style="1" customWidth="1"/>
-    <col min="392" max="392" width="15.6640625" style="4" customWidth="1"/>
-    <col min="393" max="393" width="4.6640625" style="1" customWidth="1"/>
-    <col min="394" max="394" width="15.6640625" style="4" customWidth="1"/>
-    <col min="395" max="395" width="3.6640625" style="1" customWidth="1"/>
-    <col min="396" max="396" width="15.6640625" style="4" customWidth="1"/>
-    <col min="397" max="397" width="3.6640625" style="13" customWidth="1"/>
-    <col min="398" max="398" width="18.44140625" style="12" customWidth="1"/>
-    <col min="399" max="399" width="5.88671875" style="4" customWidth="1"/>
+    <col min="380" max="380" width="17.28515625" style="4" customWidth="1"/>
+    <col min="381" max="381" width="4.85546875" style="1" customWidth="1"/>
+    <col min="382" max="382" width="15.7109375" style="4" customWidth="1"/>
+    <col min="383" max="383" width="3.7109375" style="13" customWidth="1"/>
+    <col min="384" max="384" width="18.5703125" style="12" customWidth="1"/>
+    <col min="385" max="385" width="4.85546875" style="4" customWidth="1"/>
+    <col min="386" max="386" width="15.7109375" style="12" customWidth="1"/>
+    <col min="387" max="387" width="3.7109375" style="1" customWidth="1"/>
+    <col min="388" max="388" width="15.7109375" style="4" customWidth="1"/>
+    <col min="389" max="389" width="5.42578125" style="1" customWidth="1"/>
+    <col min="390" max="390" width="15.7109375" style="4" customWidth="1"/>
+    <col min="391" max="391" width="3.7109375" style="1" customWidth="1"/>
+    <col min="392" max="392" width="15.7109375" style="4" customWidth="1"/>
+    <col min="393" max="393" width="4.7109375" style="1" customWidth="1"/>
+    <col min="394" max="394" width="15.7109375" style="4" customWidth="1"/>
+    <col min="395" max="395" width="3.7109375" style="1" customWidth="1"/>
+    <col min="396" max="396" width="15.7109375" style="4" customWidth="1"/>
+    <col min="397" max="397" width="3.7109375" style="13" customWidth="1"/>
+    <col min="398" max="398" width="18.42578125" style="12" customWidth="1"/>
+    <col min="399" max="399" width="5.85546875" style="4" customWidth="1"/>
     <col min="400" max="400" width="17" style="12" customWidth="1"/>
-    <col min="401" max="401" width="3.6640625" style="1" customWidth="1"/>
-    <col min="402" max="402" width="18.44140625" style="4" customWidth="1"/>
+    <col min="401" max="401" width="3.7109375" style="1" customWidth="1"/>
+    <col min="402" max="402" width="18.42578125" style="4" customWidth="1"/>
     <col min="403" max="403" width="5" style="1" customWidth="1"/>
-    <col min="404" max="404" width="15.6640625" style="4" customWidth="1"/>
-    <col min="405" max="405" width="3.6640625" style="1" customWidth="1"/>
-    <col min="406" max="406" width="15.6640625" style="4" customWidth="1"/>
-    <col min="407" max="407" width="3.6640625" style="1" customWidth="1"/>
-    <col min="408" max="408" width="15.6640625" style="4" customWidth="1"/>
-    <col min="409" max="409" width="3.6640625" style="1" customWidth="1"/>
-    <col min="410" max="410" width="15.6640625" style="4" customWidth="1"/>
-    <col min="411" max="411" width="3.6640625" style="13" customWidth="1"/>
+    <col min="404" max="404" width="15.7109375" style="4" customWidth="1"/>
+    <col min="405" max="405" width="3.7109375" style="1" customWidth="1"/>
+    <col min="406" max="406" width="15.7109375" style="4" customWidth="1"/>
+    <col min="407" max="407" width="3.7109375" style="1" customWidth="1"/>
+    <col min="408" max="408" width="15.7109375" style="4" customWidth="1"/>
+    <col min="409" max="409" width="3.7109375" style="1" customWidth="1"/>
+    <col min="410" max="410" width="15.7109375" style="4" customWidth="1"/>
+    <col min="411" max="411" width="3.7109375" style="13" customWidth="1"/>
     <col min="412" max="412" width="19" style="12" customWidth="1"/>
-    <col min="413" max="413" width="3.6640625" style="4" customWidth="1"/>
-    <col min="414" max="414" width="17.33203125" style="12" customWidth="1"/>
+    <col min="413" max="413" width="3.7109375" style="4" customWidth="1"/>
+    <col min="414" max="414" width="17.28515625" style="12" customWidth="1"/>
     <col min="415" max="415" width="5" style="1" customWidth="1"/>
-    <col min="416" max="416" width="15.6640625" style="4" customWidth="1"/>
-    <col min="417" max="417" width="4.33203125" style="1" customWidth="1"/>
-    <col min="418" max="418" width="15.6640625" style="4" customWidth="1"/>
-    <col min="419" max="419" width="3.6640625" style="1" customWidth="1"/>
-    <col min="420" max="420" width="15.6640625" style="4" customWidth="1"/>
-    <col min="421" max="421" width="4.88671875" style="1" customWidth="1"/>
-    <col min="422" max="422" width="15.6640625" style="4" customWidth="1"/>
-    <col min="423" max="423" width="5.88671875" style="1" customWidth="1"/>
-    <col min="424" max="424" width="15.6640625" style="4" customWidth="1"/>
-    <col min="425" max="425" width="3.6640625" style="13" customWidth="1"/>
-    <col min="426" max="426" width="18.44140625" style="12" customWidth="1"/>
-    <col min="427" max="427" width="4.88671875" style="4" customWidth="1"/>
-    <col min="428" max="428" width="17.6640625" style="12" customWidth="1"/>
-    <col min="429" max="429" width="3.6640625" style="1" customWidth="1"/>
-    <col min="430" max="430" width="15.6640625" style="4" customWidth="1"/>
-    <col min="431" max="431" width="3.6640625" style="1" customWidth="1"/>
-    <col min="432" max="432" width="15.6640625" style="4" customWidth="1"/>
-    <col min="433" max="433" width="3.6640625" style="1" customWidth="1"/>
-    <col min="434" max="434" width="15.6640625" style="4" customWidth="1"/>
-    <col min="435" max="435" width="3.6640625" style="1" customWidth="1"/>
-    <col min="436" max="436" width="15.6640625" style="4" customWidth="1"/>
-    <col min="437" max="437" width="3.6640625" style="1" customWidth="1"/>
-    <col min="438" max="438" width="15.6640625" style="4" customWidth="1"/>
-    <col min="439" max="439" width="3.6640625" style="13" customWidth="1"/>
-    <col min="440" max="440" width="18.5546875" style="12" customWidth="1"/>
-    <col min="441" max="441" width="3.6640625" style="4" customWidth="1"/>
-    <col min="442" max="442" width="19.109375" style="12" customWidth="1"/>
-    <col min="443" max="443" width="3.6640625" style="1" customWidth="1"/>
-    <col min="444" max="444" width="15.6640625" style="4" customWidth="1"/>
-    <col min="445" max="445" width="3.6640625" style="1" customWidth="1"/>
-    <col min="446" max="446" width="15.6640625" style="4" customWidth="1"/>
-    <col min="447" max="447" width="3.6640625" style="1" customWidth="1"/>
-    <col min="448" max="448" width="15.6640625" style="4" customWidth="1"/>
-    <col min="449" max="449" width="3.6640625" style="1" customWidth="1"/>
-    <col min="450" max="450" width="15.6640625" style="4" customWidth="1"/>
-    <col min="451" max="451" width="3.6640625" style="1" customWidth="1"/>
-    <col min="452" max="452" width="15.109375" style="4" customWidth="1"/>
-    <col min="453" max="453" width="3.6640625" style="13" customWidth="1"/>
+    <col min="416" max="416" width="15.7109375" style="4" customWidth="1"/>
+    <col min="417" max="417" width="4.28515625" style="1" customWidth="1"/>
+    <col min="418" max="418" width="15.7109375" style="4" customWidth="1"/>
+    <col min="419" max="419" width="3.7109375" style="1" customWidth="1"/>
+    <col min="420" max="420" width="15.7109375" style="4" customWidth="1"/>
+    <col min="421" max="421" width="4.85546875" style="1" customWidth="1"/>
+    <col min="422" max="422" width="15.7109375" style="4" customWidth="1"/>
+    <col min="423" max="423" width="5.85546875" style="1" customWidth="1"/>
+    <col min="424" max="424" width="15.7109375" style="4" customWidth="1"/>
+    <col min="425" max="425" width="3.7109375" style="13" customWidth="1"/>
+    <col min="426" max="426" width="18.42578125" style="12" customWidth="1"/>
+    <col min="427" max="427" width="4.85546875" style="4" customWidth="1"/>
+    <col min="428" max="428" width="17.7109375" style="12" customWidth="1"/>
+    <col min="429" max="429" width="3.7109375" style="1" customWidth="1"/>
+    <col min="430" max="430" width="15.7109375" style="4" customWidth="1"/>
+    <col min="431" max="431" width="3.7109375" style="1" customWidth="1"/>
+    <col min="432" max="432" width="15.7109375" style="4" customWidth="1"/>
+    <col min="433" max="433" width="3.7109375" style="1" customWidth="1"/>
+    <col min="434" max="434" width="15.7109375" style="4" customWidth="1"/>
+    <col min="435" max="435" width="3.7109375" style="1" customWidth="1"/>
+    <col min="436" max="436" width="15.7109375" style="4" customWidth="1"/>
+    <col min="437" max="437" width="3.7109375" style="1" customWidth="1"/>
+    <col min="438" max="438" width="15.7109375" style="4" customWidth="1"/>
+    <col min="439" max="439" width="3.7109375" style="13" customWidth="1"/>
+    <col min="440" max="440" width="18.5703125" style="12" customWidth="1"/>
+    <col min="441" max="441" width="3.7109375" style="4" customWidth="1"/>
+    <col min="442" max="442" width="19.140625" style="12" customWidth="1"/>
+    <col min="443" max="443" width="3.7109375" style="1" customWidth="1"/>
+    <col min="444" max="444" width="15.7109375" style="4" customWidth="1"/>
+    <col min="445" max="445" width="3.7109375" style="1" customWidth="1"/>
+    <col min="446" max="446" width="15.7109375" style="4" customWidth="1"/>
+    <col min="447" max="447" width="3.7109375" style="1" customWidth="1"/>
+    <col min="448" max="448" width="15.7109375" style="4" customWidth="1"/>
+    <col min="449" max="449" width="3.7109375" style="1" customWidth="1"/>
+    <col min="450" max="450" width="15.7109375" style="4" customWidth="1"/>
+    <col min="451" max="451" width="3.7109375" style="1" customWidth="1"/>
+    <col min="452" max="452" width="15.140625" style="4" customWidth="1"/>
+    <col min="453" max="453" width="3.7109375" style="13" customWidth="1"/>
     <col min="454" max="454" width="17" style="12" customWidth="1"/>
-    <col min="455" max="455" width="3.6640625" style="4" customWidth="1"/>
-    <col min="456" max="456" width="15.6640625" style="12" customWidth="1"/>
-    <col min="457" max="457" width="3.6640625" style="1" customWidth="1"/>
-    <col min="458" max="458" width="15.6640625" style="4" customWidth="1"/>
-    <col min="459" max="459" width="3.6640625" style="1" customWidth="1"/>
-    <col min="460" max="460" width="15.6640625" style="4" customWidth="1"/>
-    <col min="461" max="461" width="3.6640625" style="1" customWidth="1"/>
-    <col min="462" max="462" width="15.6640625" style="4" customWidth="1"/>
-    <col min="463" max="463" width="3.6640625" style="1" customWidth="1"/>
-    <col min="464" max="464" width="15.6640625" style="4" customWidth="1"/>
-    <col min="465" max="465" width="3.6640625" style="1" customWidth="1"/>
-    <col min="466" max="466" width="15.6640625" style="4" customWidth="1"/>
-    <col min="467" max="467" width="3.6640625" style="13" customWidth="1"/>
-    <col min="468" max="468" width="13.6640625" style="12" customWidth="1"/>
-    <col min="469" max="469" width="3.6640625" style="4" customWidth="1"/>
-    <col min="470" max="470" width="17.109375" style="12" customWidth="1"/>
-    <col min="471" max="471" width="3.6640625" style="1" customWidth="1"/>
-    <col min="472" max="472" width="15.6640625" style="4" customWidth="1"/>
-    <col min="473" max="473" width="3.6640625" style="1" customWidth="1"/>
-    <col min="474" max="474" width="15.6640625" style="4" customWidth="1"/>
-    <col min="475" max="475" width="3.6640625" style="1" customWidth="1"/>
-    <col min="476" max="476" width="15.6640625" style="4" customWidth="1"/>
-    <col min="477" max="477" width="3.6640625" style="1" customWidth="1"/>
-    <col min="478" max="478" width="15.6640625" style="4" customWidth="1"/>
-    <col min="479" max="479" width="3.6640625" style="1" customWidth="1"/>
-    <col min="480" max="480" width="17.33203125" style="4" customWidth="1"/>
-    <col min="481" max="481" width="3.6640625" style="13" customWidth="1"/>
-    <col min="482" max="16384" width="3.6640625" style="13"/>
+    <col min="455" max="455" width="3.7109375" style="4" customWidth="1"/>
+    <col min="456" max="456" width="15.7109375" style="12" customWidth="1"/>
+    <col min="457" max="457" width="3.7109375" style="1" customWidth="1"/>
+    <col min="458" max="458" width="15.7109375" style="4" customWidth="1"/>
+    <col min="459" max="459" width="3.7109375" style="1" customWidth="1"/>
+    <col min="460" max="460" width="15.7109375" style="4" customWidth="1"/>
+    <col min="461" max="461" width="3.7109375" style="1" customWidth="1"/>
+    <col min="462" max="462" width="15.7109375" style="4" customWidth="1"/>
+    <col min="463" max="463" width="3.7109375" style="1" customWidth="1"/>
+    <col min="464" max="464" width="15.7109375" style="4" customWidth="1"/>
+    <col min="465" max="465" width="3.7109375" style="1" customWidth="1"/>
+    <col min="466" max="466" width="15.7109375" style="4" customWidth="1"/>
+    <col min="467" max="467" width="3.7109375" style="13" customWidth="1"/>
+    <col min="468" max="468" width="13.7109375" style="12" customWidth="1"/>
+    <col min="469" max="469" width="3.7109375" style="4" customWidth="1"/>
+    <col min="470" max="470" width="17.140625" style="12" customWidth="1"/>
+    <col min="471" max="471" width="3.7109375" style="1" customWidth="1"/>
+    <col min="472" max="472" width="15.7109375" style="4" customWidth="1"/>
+    <col min="473" max="473" width="3.7109375" style="1" customWidth="1"/>
+    <col min="474" max="474" width="15.7109375" style="4" customWidth="1"/>
+    <col min="475" max="475" width="3.7109375" style="1" customWidth="1"/>
+    <col min="476" max="476" width="15.7109375" style="4" customWidth="1"/>
+    <col min="477" max="477" width="3.7109375" style="1" customWidth="1"/>
+    <col min="478" max="478" width="15.7109375" style="4" customWidth="1"/>
+    <col min="479" max="479" width="3.7109375" style="1" customWidth="1"/>
+    <col min="480" max="480" width="17.28515625" style="4" customWidth="1"/>
+    <col min="481" max="481" width="3.7109375" style="13" customWidth="1"/>
+    <col min="482" max="16384" width="3.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:481" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:481" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -9695,7 +9701,7 @@
       <c r="RL1" s="45"/>
       <c r="RM1" s="46"/>
     </row>
-    <row r="2" spans="1:481" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:481" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="47" t="s">
         <v>62</v>
       </c>
@@ -10177,7 +10183,7 @@
       <c r="RL2" s="45"/>
       <c r="RM2" s="46"/>
     </row>
-    <row r="3" spans="1:481" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:481" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" s="6"/>
       <c r="D3"/>
@@ -11134,7 +11140,7 @@
       </c>
       <c r="RM3" s="19"/>
     </row>
-    <row r="4" spans="1:481" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:481" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="b">
         <f>AND(LEN($F$5)&gt;1,LEN($G$5)=0)</f>
         <v>0</v>
@@ -12338,7 +12344,7 @@
       </c>
       <c r="RM4" s="23"/>
     </row>
-    <row r="5" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>91</v>
       </c>
@@ -12798,7 +12804,7 @@
       <c r="RK5" s="13"/>
       <c r="RL5" s="14"/>
     </row>
-    <row r="6" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>92</v>
       </c>
@@ -13298,7 +13304,7 @@
       <c r="RL6" s="14"/>
       <c r="RM6" s="13"/>
     </row>
-    <row r="7" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>92</v>
       </c>
@@ -13798,7 +13804,7 @@
       <c r="RL7" s="14"/>
       <c r="RM7" s="13"/>
     </row>
-    <row r="8" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>93</v>
       </c>
@@ -14317,7 +14323,7 @@
       <c r="RL8" s="14"/>
       <c r="RM8" s="13"/>
     </row>
-    <row r="9" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>93</v>
       </c>
@@ -14835,7 +14841,7 @@
       <c r="RL9" s="14"/>
       <c r="RM9" s="13"/>
     </row>
-    <row r="10" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>93</v>
       </c>
@@ -15347,7 +15353,7 @@
       <c r="RL10" s="14"/>
       <c r="RM10" s="13"/>
     </row>
-    <row r="11" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>93</v>
       </c>
@@ -15857,7 +15863,7 @@
       <c r="RL11" s="14"/>
       <c r="RM11" s="13"/>
     </row>
-    <row r="12" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>93</v>
       </c>
@@ -16367,7 +16373,7 @@
       <c r="RL12" s="14"/>
       <c r="RM12" s="13"/>
     </row>
-    <row r="13" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>93</v>
       </c>
@@ -16835,7 +16841,7 @@
       <c r="RK13" s="13"/>
       <c r="RL13" s="14"/>
     </row>
-    <row r="14" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>98</v>
       </c>
@@ -17329,7 +17335,7 @@
       <c r="RK14" s="13"/>
       <c r="RL14" s="14"/>
     </row>
-    <row r="15" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>98</v>
       </c>
@@ -17823,7 +17829,7 @@
       <c r="RK15" s="13"/>
       <c r="RL15" s="14"/>
     </row>
-    <row r="16" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>98</v>
       </c>
@@ -18315,7 +18321,7 @@
       <c r="RK16" s="13"/>
       <c r="RL16" s="14"/>
     </row>
-    <row r="17" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>98</v>
       </c>
@@ -18805,7 +18811,7 @@
       <c r="RK17" s="13"/>
       <c r="RL17" s="14"/>
     </row>
-    <row r="18" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>94</v>
       </c>
@@ -19323,7 +19329,7 @@
       <c r="RL18" s="14"/>
       <c r="RM18" s="13"/>
     </row>
-    <row r="19" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>94</v>
       </c>
@@ -19855,7 +19861,7 @@
       <c r="RL19" s="14"/>
       <c r="RM19" s="13"/>
     </row>
-    <row r="20" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>94</v>
       </c>
@@ -20381,7 +20387,7 @@
       <c r="RL20" s="14"/>
       <c r="RM20" s="13"/>
     </row>
-    <row r="21" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>94</v>
       </c>
@@ -20871,7 +20877,7 @@
       <c r="RK21" s="13"/>
       <c r="RL21" s="14"/>
     </row>
-    <row r="22" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>95</v>
       </c>
@@ -21406,7 +21412,7 @@
       <c r="RL22" s="14"/>
       <c r="RM22" s="13"/>
     </row>
-    <row r="23" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>95</v>
       </c>
@@ -21942,7 +21948,7 @@
       <c r="RL23" s="14"/>
       <c r="RM23" s="13"/>
     </row>
-    <row r="24" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>95</v>
       </c>
@@ -22468,7 +22474,7 @@
       <c r="RL24" s="14"/>
       <c r="RM24" s="13"/>
     </row>
-    <row r="25" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>95</v>
       </c>
@@ -22992,7 +22998,7 @@
       <c r="RL25" s="14"/>
       <c r="RM25" s="13"/>
     </row>
-    <row r="26" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>95</v>
       </c>
@@ -23518,7 +23524,7 @@
       <c r="RL26" s="14"/>
       <c r="RM26" s="13"/>
     </row>
-    <row r="27" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>95</v>
       </c>
@@ -24046,7 +24052,7 @@
       <c r="RL27" s="14"/>
       <c r="RM27" s="13"/>
     </row>
-    <row r="28" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>95</v>
       </c>
@@ -24531,7 +24537,7 @@
       <c r="RK28" s="13"/>
       <c r="RL28" s="14"/>
     </row>
-    <row r="29" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>96</v>
       </c>
@@ -25071,7 +25077,7 @@
       <c r="RL29" s="14"/>
       <c r="RM29" s="13"/>
     </row>
-    <row r="30" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
         <v>96</v>
       </c>
@@ -25609,7 +25615,7 @@
       <c r="RL30" s="14"/>
       <c r="RM30" s="13"/>
     </row>
-    <row r="31" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>96</v>
       </c>
@@ -26161,7 +26167,7 @@
       <c r="RL31" s="14"/>
       <c r="RM31" s="13"/>
     </row>
-    <row r="32" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
         <v>96</v>
       </c>
@@ -26705,7 +26711,7 @@
       <c r="RL32" s="14"/>
       <c r="RM32" s="13"/>
     </row>
-    <row r="33" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
         <v>96</v>
       </c>
@@ -27227,7 +27233,7 @@
       <c r="RL33" s="14"/>
       <c r="RM33" s="13"/>
     </row>
-    <row r="34" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:481" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
         <v>97</v>
       </c>
@@ -27734,7 +27740,7 @@
       <c r="RK34" s="13"/>
       <c r="RL34" s="14"/>
     </row>
-    <row r="35" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:481" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
         <v>97</v>
       </c>
@@ -28284,7 +28290,7 @@
       <c r="RL35" s="14"/>
       <c r="RM35" s="13"/>
     </row>
-    <row r="36" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
         <v>97</v>
       </c>
@@ -28828,7 +28834,7 @@
       <c r="RL36" s="14"/>
       <c r="RM36" s="13"/>
     </row>
-    <row r="37" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:481" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
         <v>97</v>
       </c>
@@ -29350,7 +29356,7 @@
       <c r="RL37" s="14"/>
       <c r="RM37" s="13"/>
     </row>
-    <row r="38" spans="1:481" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:481" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="32" t="s">
         <v>128</v>
       </c>
@@ -29560,10 +29566,18 @@
       <c r="FN38" s="14"/>
       <c r="FO38" s="13"/>
       <c r="FP38" s="14"/>
-      <c r="FR38" s="14"/>
-      <c r="FS38" s="13"/>
-      <c r="FT38" s="14"/>
-      <c r="FU38" s="13"/>
+      <c r="FR38" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="FS38" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="FT38" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="FU38" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="FV38" s="14" t="s">
         <v>102</v>
       </c>
@@ -29895,7 +29909,7 @@
       <c r="RK38" s="13"/>
       <c r="RL38" s="14"/>
     </row>
-    <row r="39" spans="1:481" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:481" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="25"/>
       <c r="C39" s="10"/>
       <c r="D39" s="9"/>
@@ -30343,7 +30357,7 @@
       <c r="RK39" s="13"/>
       <c r="RL39" s="14"/>
     </row>
-    <row r="40" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>19</v>
       </c>
@@ -31028,7 +31042,7 @@
       </c>
       <c r="RM40" s="17"/>
     </row>
-    <row r="41" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:481" x14ac:dyDescent="0.25">
       <c r="F41" s="12" t="s">
         <v>12</v>
       </c>
@@ -31982,7 +31996,7 @@
       </c>
       <c r="RM41" s="17"/>
     </row>
-    <row r="42" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:481" x14ac:dyDescent="0.25">
       <c r="F42" s="12" t="s">
         <v>14</v>
       </c>
@@ -32936,7 +32950,7 @@
       </c>
       <c r="RM42" s="17"/>
     </row>
-    <row r="43" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:481" x14ac:dyDescent="0.25">
       <c r="G43" s="1"/>
       <c r="H43" s="28"/>
       <c r="J43" s="28"/>
@@ -33731,7 +33745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>11</v>
       </c>
@@ -34199,7 +34213,7 @@
       </c>
       <c r="FU44" s="13">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FV44" s="28" t="s">
         <v>120</v>
@@ -34524,7 +34538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B45" s="42">
         <v>1</v>
       </c>
@@ -35276,7 +35290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B46" s="42">
         <v>0.5</v>
       </c>
@@ -35953,7 +35967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B47" s="42" t="s">
         <v>8</v>
       </c>
@@ -36347,7 +36361,7 @@
       </c>
       <c r="FS47" s="13">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FT47" s="28" t="s">
         <v>63</v>
@@ -36626,7 +36640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:481" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:481" x14ac:dyDescent="0.25">
       <c r="B48" s="42" t="s">
         <v>9</v>
       </c>
@@ -37280,7 +37294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:481" x14ac:dyDescent="0.25">
       <c r="B49" s="42" t="s">
         <v>10</v>
       </c>
@@ -37898,7 +37912,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:481" x14ac:dyDescent="0.25">
+      <c r="B50" s="42" t="s">
+        <v>157</v>
+      </c>
       <c r="H50" s="28"/>
       <c r="S50" s="13">
         <f t="shared" si="5"/>
@@ -38516,7 +38533,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:481" x14ac:dyDescent="0.25">
+      <c r="B51" s="42" t="s">
+        <v>158</v>
+      </c>
       <c r="F51" s="27"/>
       <c r="H51" s="28"/>
       <c r="S51" s="13">
@@ -39135,7 +39155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:481" x14ac:dyDescent="0.25">
       <c r="F52" s="27"/>
       <c r="H52" s="28"/>
       <c r="S52" s="13">
@@ -39749,7 +39769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H53" s="28"/>
       <c r="S53" s="13">
         <f t="shared" si="5"/>
@@ -40357,7 +40377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H54" s="28"/>
       <c r="S54" s="13">
         <f t="shared" si="5"/>
@@ -40963,7 +40983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H55" s="28"/>
       <c r="S55" s="13">
         <f t="shared" si="5"/>
@@ -41557,7 +41577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H56" s="28"/>
       <c r="S56" s="13">
         <f t="shared" si="5"/>
@@ -42128,7 +42148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H57" s="28"/>
       <c r="S57" s="13">
         <f t="shared" si="5"/>
@@ -42680,7 +42700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="S58" s="13">
         <f t="shared" si="5"/>
@@ -43215,7 +43235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="S59" s="13">
         <f t="shared" si="5"/>
@@ -43752,7 +43772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:481" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="S60" s="13">
         <f t="shared" si="5"/>
@@ -44289,7 +44309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:481" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>20</v>
       </c>
@@ -45065,7 +45085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:481" x14ac:dyDescent="0.25">
       <c r="NI62" s="1">
         <f>COUNTIF(NH$5:NH$39,NH57)</f>
         <v>0</v>
@@ -45095,7 +45115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:481" x14ac:dyDescent="0.25">
       <c r="NI63" s="1">
         <f>COUNTIF(NH$5:NH$39,NH58)</f>
         <v>0</v>
@@ -45109,7 +45129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:481" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:481" x14ac:dyDescent="0.25">
       <c r="NI64" s="1">
         <f>COUNTIF(NH$5:NH$39,NH59)</f>
         <v>0</v>
@@ -45123,7 +45143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:427" x14ac:dyDescent="0.25">
       <c r="CX65" s="4">
         <f>COUNTA(CP43:CX60)</f>
         <v>73</v>
@@ -45169,13 +45189,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:427" x14ac:dyDescent="0.25">
       <c r="PK66" s="4">
         <f t="shared" si="137"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:427" ht="27" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:427" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>91</v>
       </c>
@@ -45191,7 +45211,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="70" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A70" s="43" t="s">
         <v>92</v>
       </c>
@@ -45213,7 +45233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
         <v>92</v>
       </c>
@@ -45231,7 +45251,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="72" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
         <v>93</v>
       </c>
@@ -45247,7 +45267,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="73" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A73" s="41" t="s">
         <v>93</v>
       </c>
@@ -45259,7 +45279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="s">
         <v>93</v>
       </c>
@@ -45277,7 +45297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
         <v>93</v>
       </c>
@@ -45295,7 +45315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A76" s="40" t="s">
         <v>93</v>
       </c>
@@ -45313,7 +45333,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:427" ht="27" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:427" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="40" t="s">
         <v>93</v>
       </c>
@@ -45325,7 +45345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:427" ht="27" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:427" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
         <v>98</v>
       </c>
@@ -45343,7 +45363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:427" ht="27" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:427" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
         <v>98</v>
       </c>
@@ -45361,7 +45381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:427" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:427" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
         <v>98</v>
       </c>
@@ -45379,7 +45399,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
         <v>98</v>
       </c>
@@ -45391,7 +45411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="s">
         <v>94</v>
       </c>
@@ -45409,7 +45429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
         <v>94</v>
       </c>
@@ -45427,7 +45447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A84" s="34" t="s">
         <v>94</v>
       </c>
@@ -45447,7 +45467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A85" s="34" t="s">
         <v>94</v>
       </c>
@@ -45461,7 +45481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A86" s="35" t="s">
         <v>95</v>
       </c>
@@ -45481,7 +45501,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="87" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A87" s="35" t="s">
         <v>95</v>
       </c>
@@ -45495,7 +45515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A88" s="35" t="s">
         <v>95</v>
       </c>
@@ -45509,7 +45529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A89" s="35" t="s">
         <v>95</v>
       </c>
@@ -45523,7 +45543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A90" s="38" t="s">
         <v>95</v>
       </c>
@@ -45537,7 +45557,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="91" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A91" s="38" t="s">
         <v>95</v>
       </c>
@@ -45551,7 +45571,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="92" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A92" s="38" t="s">
         <v>95</v>
       </c>
@@ -45565,7 +45585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A93" s="36" t="s">
         <v>96</v>
       </c>
@@ -45579,7 +45599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
         <v>96</v>
       </c>
@@ -45593,7 +45613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>96</v>
       </c>
@@ -45607,7 +45627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:252" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:252" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
         <v>96</v>
       </c>
@@ -45621,7 +45641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A97" s="39" t="s">
         <v>96</v>
       </c>
@@ -45635,7 +45655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
         <v>97</v>
       </c>
@@ -45649,7 +45669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A99" s="37" t="s">
         <v>97</v>
       </c>
@@ -45663,7 +45683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A100" s="37" t="s">
         <v>97</v>
       </c>
@@ -45677,7 +45697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:108" ht="27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:108" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="39" t="s">
         <v>97</v>
       </c>
@@ -45691,22 +45711,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:108" x14ac:dyDescent="0.25">
       <c r="D102" s="11"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:108" x14ac:dyDescent="0.25">
       <c r="D103" s="11"/>
       <c r="E103" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="QZ1:RM1"/>
-    <mergeCell ref="QZ2:RM2"/>
-    <mergeCell ref="PJ2:PW2"/>
-    <mergeCell ref="PX2:QK2"/>
-    <mergeCell ref="QL1:QY1"/>
-    <mergeCell ref="QL2:QY2"/>
+    <mergeCell ref="IJ1:IW1"/>
+    <mergeCell ref="IJ2:IW2"/>
+    <mergeCell ref="GF2:GS2"/>
+    <mergeCell ref="GT2:HG2"/>
+    <mergeCell ref="HH2:HU2"/>
+    <mergeCell ref="HV2:II2"/>
+    <mergeCell ref="GF1:GS1"/>
+    <mergeCell ref="GT1:HG1"/>
+    <mergeCell ref="HH1:HU1"/>
+    <mergeCell ref="HV1:II1"/>
+    <mergeCell ref="FR2:GE2"/>
+    <mergeCell ref="EB1:EO1"/>
+    <mergeCell ref="EP1:FC1"/>
+    <mergeCell ref="FD1:FQ1"/>
+    <mergeCell ref="FR1:GE1"/>
+    <mergeCell ref="EB2:EO2"/>
+    <mergeCell ref="EP2:FC2"/>
+    <mergeCell ref="CZ1:DM1"/>
+    <mergeCell ref="DN1:EA1"/>
+    <mergeCell ref="AH1:AU1"/>
+    <mergeCell ref="AH2:AU2"/>
+    <mergeCell ref="FD2:FQ2"/>
+    <mergeCell ref="BX2:CK2"/>
+    <mergeCell ref="CL2:CY2"/>
+    <mergeCell ref="CZ2:DM2"/>
+    <mergeCell ref="DN2:EA2"/>
+    <mergeCell ref="CL1:CY1"/>
+    <mergeCell ref="AV1:BI1"/>
+    <mergeCell ref="BJ1:BW1"/>
+    <mergeCell ref="AV2:BI2"/>
+    <mergeCell ref="BJ2:BW2"/>
+    <mergeCell ref="F1:S1"/>
+    <mergeCell ref="F2:S2"/>
+    <mergeCell ref="T1:AG1"/>
+    <mergeCell ref="T2:AG2"/>
+    <mergeCell ref="BX1:CK1"/>
+    <mergeCell ref="IX1:JK1"/>
+    <mergeCell ref="JL1:JY1"/>
+    <mergeCell ref="JZ1:KM1"/>
+    <mergeCell ref="KN1:LA1"/>
+    <mergeCell ref="LB1:LO1"/>
+    <mergeCell ref="LP1:MC1"/>
+    <mergeCell ref="MD1:MQ1"/>
+    <mergeCell ref="MR1:NE1"/>
+    <mergeCell ref="NF1:NS1"/>
+    <mergeCell ref="NT1:OG1"/>
     <mergeCell ref="OH1:OU1"/>
     <mergeCell ref="OV1:PI1"/>
     <mergeCell ref="PJ1:PW1"/>
@@ -45723,52 +45783,12 @@
     <mergeCell ref="NT2:OG2"/>
     <mergeCell ref="OH2:OU2"/>
     <mergeCell ref="OV2:PI2"/>
-    <mergeCell ref="LP1:MC1"/>
-    <mergeCell ref="MD1:MQ1"/>
-    <mergeCell ref="MR1:NE1"/>
-    <mergeCell ref="NF1:NS1"/>
-    <mergeCell ref="NT1:OG1"/>
-    <mergeCell ref="IX1:JK1"/>
-    <mergeCell ref="JL1:JY1"/>
-    <mergeCell ref="JZ1:KM1"/>
-    <mergeCell ref="KN1:LA1"/>
-    <mergeCell ref="LB1:LO1"/>
-    <mergeCell ref="F1:S1"/>
-    <mergeCell ref="F2:S2"/>
-    <mergeCell ref="T1:AG1"/>
-    <mergeCell ref="T2:AG2"/>
-    <mergeCell ref="BX1:CK1"/>
-    <mergeCell ref="CZ1:DM1"/>
-    <mergeCell ref="DN1:EA1"/>
-    <mergeCell ref="AH1:AU1"/>
-    <mergeCell ref="AH2:AU2"/>
-    <mergeCell ref="FD2:FQ2"/>
-    <mergeCell ref="BX2:CK2"/>
-    <mergeCell ref="CL2:CY2"/>
-    <mergeCell ref="CZ2:DM2"/>
-    <mergeCell ref="DN2:EA2"/>
-    <mergeCell ref="CL1:CY1"/>
-    <mergeCell ref="AV1:BI1"/>
-    <mergeCell ref="BJ1:BW1"/>
-    <mergeCell ref="AV2:BI2"/>
-    <mergeCell ref="BJ2:BW2"/>
-    <mergeCell ref="FR2:GE2"/>
-    <mergeCell ref="EB1:EO1"/>
-    <mergeCell ref="EP1:FC1"/>
-    <mergeCell ref="FD1:FQ1"/>
-    <mergeCell ref="FR1:GE1"/>
-    <mergeCell ref="EB2:EO2"/>
-    <mergeCell ref="EP2:FC2"/>
-    <mergeCell ref="IJ1:IW1"/>
-    <mergeCell ref="IJ2:IW2"/>
-    <mergeCell ref="GF2:GS2"/>
-    <mergeCell ref="GT2:HG2"/>
-    <mergeCell ref="HH2:HU2"/>
-    <mergeCell ref="HV2:II2"/>
-    <mergeCell ref="GF1:GS1"/>
-    <mergeCell ref="GT1:HG1"/>
-    <mergeCell ref="HH1:HU1"/>
-    <mergeCell ref="HV1:II1"/>
+    <mergeCell ref="QZ1:RM1"/>
+    <mergeCell ref="QZ2:RM2"/>
+    <mergeCell ref="PJ2:PW2"/>
+    <mergeCell ref="PX2:QK2"/>
+    <mergeCell ref="QL1:QY1"/>
+    <mergeCell ref="QL2:QY2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N46:N47 L43:L60 R43:R60 P46:P60 F43:F50 H47:H60 N49:N60 F53:F60 J45:J60 FR57:FR60 OH43:OH50 OV43:OV50 NH43:NH44 BZ59:BZ60 BL57:BL58 BL60 GH57:GH60 GF57:GF60 HH57:HH60 JZ43:JZ52 JZ55 MD43:MD52 MD55 MR43:MR52 MR55 NF43:NF52 NF55 HJ57:HJ60 MF43:MF48 MF52:MF55 PL54:PL57 PL59:PL60 BF46 BD47:BD60 BF48:BF60 DR43:DR56 DR59:DR60 EB56:EB60 EB43:EB53 ED57:ED60 ED53:ED54">
@@ -51100,7 +51120,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -51113,7 +51133,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -51126,7 +51146,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Almost all changes for web version.
</commit_message>
<xml_diff>
--- a/RingetteSchedule/Master.xlsx
+++ b/RingetteSchedule/Master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A57BF290-A40D-4B3F-A38F-B0B2CC8EE112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F6B8EB-752E-449E-A73E-DA09F005E53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="163" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="163" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="175">
   <si>
     <t>Sat</t>
   </si>
@@ -9210,10 +9210,10 @@
   <dimension ref="A1:RO103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="II11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="ID20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="IM27" sqref="IM27"/>
+      <selection pane="bottomRight" activeCell="IL22" sqref="IL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15622,7 +15622,7 @@
       </c>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
@@ -15891,12 +15891,8 @@
       <c r="HG10" s="13"/>
       <c r="HH10" s="14"/>
       <c r="HI10" s="13"/>
-      <c r="HJ10" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="HK10" s="13">
-        <v>0.5</v>
-      </c>
+      <c r="HJ10" s="14"/>
+      <c r="HK10" s="13"/>
       <c r="HL10" s="14"/>
       <c r="HM10" s="13"/>
       <c r="HN10" s="14" t="s">
@@ -22685,7 +22681,7 @@
       <c r="HZ22" s="14"/>
       <c r="IA22" s="15"/>
       <c r="IB22" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="IC22" s="15">
         <v>0.5</v>
@@ -22699,7 +22695,7 @@
       <c r="IJ22" s="14"/>
       <c r="IK22" s="13"/>
       <c r="IL22" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="IM22" s="13">
         <v>0.5</v>
@@ -23861,7 +23857,7 @@
       <c r="HZ24" s="14"/>
       <c r="IA24" s="13"/>
       <c r="IB24" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="IC24" s="13">
         <v>0.5</v>
@@ -24463,7 +24459,7 @@
       <c r="IJ25" s="14"/>
       <c r="IK25" s="13"/>
       <c r="IL25" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="IM25" s="13">
         <v>0.5</v>
@@ -38177,7 +38173,7 @@
       </c>
       <c r="HK46" s="13">
         <f t="shared" si="101"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HL46" s="28" t="s">
         <v>109</v>

</xml_diff>